<commit_message>
Atualização da tabela de comparação
</commit_message>
<xml_diff>
--- a/Arquivos/Comparações/Comparação ILS x RVND e número de pertubações.xlsx
+++ b/Arquivos/Comparações/Comparação ILS x RVND e número de pertubações.xlsx
@@ -93,13 +93,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="0_ "/>
-    <numFmt numFmtId="180" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="0_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -116,9 +116,23 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -132,6 +146,28 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -153,10 +189,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -165,51 +202,6 @@
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -226,6 +218,22 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -250,21 +258,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -275,6 +268,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -287,180 +316,144 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -480,6 +473,39 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -514,24 +540,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -556,6 +564,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -570,187 +598,167 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
@@ -759,10 +767,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1099,7 +1113,7 @@
   <dimension ref="B2:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75"/>
@@ -1115,50 +1129,50 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="8" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:18">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2" t="s">
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="5"/>
     </row>
     <row r="4" spans="2:18">
       <c r="B4" s="1" t="s">
@@ -1209,709 +1223,709 @@
       <c r="Q4" s="1">
         <v>4</v>
       </c>
-      <c r="R4" s="8"/>
+      <c r="R4" s="5"/>
     </row>
     <row r="5" ht="15" spans="2:18">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>13</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>480.48</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <v>480.48</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>480.48</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>480.48</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>480.48</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>480.48</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>480.48</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>480.48</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>480.48</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <v>480.48</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="3">
         <v>480.48</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="3">
         <v>480.48</v>
       </c>
-      <c r="P5" s="5">
+      <c r="P5" s="3">
         <v>480.48</v>
       </c>
-      <c r="Q5" s="5">
+      <c r="Q5" s="3">
         <v>480.48</v>
       </c>
-      <c r="R5" s="10">
+      <c r="R5" s="9">
         <f>SMALL(D5:Q5,1)</f>
         <v>480.48</v>
       </c>
     </row>
     <row r="6" ht="15" spans="2:18">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="2">
         <v>65</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>2541.67</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <v>2527.57</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>2590.18</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>2706.57</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>2566.81</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>2589.26</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>2585.74</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>2427.59</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>2615.61</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="3">
         <v>2566.61</v>
       </c>
-      <c r="N6" s="5">
+      <c r="N6" s="3">
         <v>2596.61</v>
       </c>
-      <c r="O6" s="5">
+      <c r="O6" s="3">
         <v>2542.27</v>
       </c>
-      <c r="P6" s="5">
+      <c r="P6" s="3">
         <v>2603.85</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="Q6" s="3">
         <v>2379.09</v>
       </c>
-      <c r="R6" s="10">
+      <c r="R6" s="9">
         <f t="shared" ref="R6:R14" si="0">SMALL(D6:Q6,1)</f>
         <v>2379.09</v>
       </c>
     </row>
     <row r="7" ht="15" spans="2:18">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>57</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>340.02</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="3">
         <v>341.64</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>337.45</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>350.58</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>348.15</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>336.82</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>337.83</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>355.1</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>348.36</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="3">
         <v>342.3</v>
       </c>
-      <c r="N7" s="5">
+      <c r="N7" s="3">
         <v>346.41</v>
       </c>
-      <c r="O7" s="5">
+      <c r="O7" s="3">
         <v>337.58</v>
       </c>
-      <c r="P7" s="5">
+      <c r="P7" s="3">
         <v>341.36</v>
       </c>
-      <c r="Q7" s="5">
+      <c r="Q7" s="3">
         <v>338.22</v>
       </c>
-      <c r="R7" s="10">
+      <c r="R7" s="9">
         <f t="shared" si="0"/>
         <v>336.82</v>
       </c>
     </row>
     <row r="8" ht="15" spans="2:18">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>150</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>20463.14</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <v>20596.28</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>20677.31</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>20544.02</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>19919.11</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>20640.9</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>19811.48</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>19981.61</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <v>20693.7</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="3">
         <v>20854.42</v>
       </c>
-      <c r="N8" s="5">
+      <c r="N8" s="3">
         <v>20657.87</v>
       </c>
-      <c r="O8" s="5">
+      <c r="O8" s="3">
         <v>20271.45</v>
       </c>
-      <c r="P8" s="5">
+      <c r="P8" s="3">
         <v>20633.36</v>
       </c>
-      <c r="Q8" s="5">
+      <c r="Q8" s="3">
         <v>20436.35</v>
       </c>
-      <c r="R8" s="10">
+      <c r="R8" s="9">
         <f t="shared" si="0"/>
         <v>19811.48</v>
       </c>
     </row>
     <row r="9" ht="15" spans="2:18">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>79</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>8598.9</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="3">
         <v>8571.87</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>10766.37</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>10778.88</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>10127.42</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>9645.45</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <v>8391.63</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <v>7982.68</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="3">
         <v>8197.11</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="3">
         <v>9155.62</v>
       </c>
-      <c r="N9" s="5">
+      <c r="N9" s="3">
         <v>11333.74</v>
       </c>
-      <c r="O9" s="5">
+      <c r="O9" s="3">
         <v>9443.92</v>
       </c>
-      <c r="P9" s="5">
+      <c r="P9" s="3">
         <v>9295.15</v>
       </c>
-      <c r="Q9" s="5">
+      <c r="Q9" s="3">
         <v>9775.26</v>
       </c>
-      <c r="R9" s="10">
+      <c r="R9" s="9">
         <f t="shared" si="0"/>
         <v>7982.68</v>
       </c>
     </row>
     <row r="10" ht="15" spans="2:18">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>109</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>19972.3</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="3">
         <v>19801.02</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>19856.75</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>18862.25</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>19347.24</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>18072.84</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>18524.67</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>17996.88</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <v>17940.83</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="3">
         <v>18405.11</v>
       </c>
-      <c r="N10" s="5">
+      <c r="N10" s="3">
         <v>19225.4</v>
       </c>
-      <c r="O10" s="5">
+      <c r="O10" s="3">
         <v>17810.85</v>
       </c>
-      <c r="P10" s="5">
+      <c r="P10" s="3">
         <v>23767.79</v>
       </c>
-      <c r="Q10" s="5">
+      <c r="Q10" s="3">
         <v>18184.34</v>
       </c>
-      <c r="R10" s="10">
+      <c r="R10" s="9">
         <f t="shared" si="0"/>
         <v>17810.85</v>
       </c>
     </row>
     <row r="11" ht="15" spans="2:18">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>87</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>10343</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="3">
         <v>10343</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>9996</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>10055</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>10029</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>9985</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>10150</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>10048</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <v>9978</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="3">
         <v>10062</v>
       </c>
-      <c r="N11" s="5">
+      <c r="N11" s="3">
         <v>9981</v>
       </c>
-      <c r="O11" s="5">
+      <c r="O11" s="3">
         <v>10065</v>
       </c>
-      <c r="P11" s="5">
+      <c r="P11" s="3">
         <v>9942</v>
       </c>
-      <c r="Q11" s="5">
+      <c r="Q11" s="3">
         <v>9901</v>
       </c>
-      <c r="R11" s="10">
+      <c r="R11" s="9">
         <f t="shared" si="0"/>
         <v>9901</v>
       </c>
     </row>
     <row r="12" ht="15" spans="2:18">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>52</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>440.64</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="3">
         <v>436.29</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>454.29</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>440.91</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>451.84</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>438.05</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>437.65</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <v>448.07</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="3">
         <v>425.5</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="3">
         <v>446.01</v>
       </c>
-      <c r="N12" s="5">
+      <c r="N12" s="3">
         <v>425.05</v>
       </c>
-      <c r="O12" s="5">
+      <c r="O12" s="3">
         <v>438.05</v>
       </c>
-      <c r="P12" s="5">
+      <c r="P12" s="3">
         <v>450.04</v>
       </c>
-      <c r="Q12" s="5">
+      <c r="Q12" s="3">
         <v>454.36</v>
       </c>
-      <c r="R12" s="10">
+      <c r="R12" s="9">
         <f t="shared" si="0"/>
         <v>425.05</v>
       </c>
     </row>
     <row r="13" ht="15" spans="2:18">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>31</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="3">
         <v>715</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="3">
         <v>715</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>698</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>698</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>721</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="3">
         <v>698</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="3">
         <v>718</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="3">
         <v>717</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="3">
         <v>698</v>
       </c>
-      <c r="M13" s="4">
+      <c r="M13" s="3">
         <v>718</v>
       </c>
-      <c r="N13" s="5">
+      <c r="N13" s="3">
         <v>721</v>
       </c>
-      <c r="O13" s="5">
+      <c r="O13" s="3">
         <v>698</v>
       </c>
-      <c r="P13" s="5">
+      <c r="P13" s="3">
         <v>746</v>
       </c>
-      <c r="Q13" s="5">
+      <c r="Q13" s="3">
         <v>698</v>
       </c>
-      <c r="R13" s="10">
+      <c r="R13" s="9">
         <f t="shared" si="0"/>
         <v>698</v>
       </c>
     </row>
     <row r="14" ht="15" spans="2:18">
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>16</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>2540.07</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="3">
         <v>2540.07</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>2540.07</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>2662.75</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <v>2540.07</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>2571.03</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="3">
         <v>2540.07</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="3">
         <v>2540.07</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="3">
         <v>2766.61</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="3">
         <v>2540.07</v>
       </c>
-      <c r="N14" s="5">
+      <c r="N14" s="3">
         <v>2540.07</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O14" s="3">
         <v>2571.03</v>
       </c>
-      <c r="P14" s="5">
+      <c r="P14" s="3">
         <v>2540.07</v>
       </c>
-      <c r="Q14" s="5">
+      <c r="Q14" s="3">
         <v>2540.07</v>
       </c>
-      <c r="R14" s="10">
+      <c r="R14" s="9">
         <f t="shared" si="0"/>
         <v>2540.07</v>
       </c>
     </row>
     <row r="15" spans="2:18">
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="7">
+      <c r="C15" s="1"/>
+      <c r="D15" s="4">
         <v>2</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="4">
         <v>2</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="4">
         <v>3</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="4">
         <v>2</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="4">
         <v>2</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="4">
         <v>3</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="4">
         <v>3</v>
       </c>
-      <c r="K15" s="7">
+      <c r="K15" s="4">
         <v>3</v>
       </c>
-      <c r="L15" s="7">
+      <c r="L15" s="4">
         <v>2</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="4">
         <v>2</v>
       </c>
-      <c r="N15" s="7">
+      <c r="N15" s="4">
         <v>3</v>
       </c>
-      <c r="O15" s="7">
+      <c r="O15" s="4">
         <v>3</v>
       </c>
-      <c r="P15" s="7">
+      <c r="P15" s="4">
         <v>2</v>
       </c>
-      <c r="Q15" s="7">
+      <c r="Q15" s="4">
         <v>5</v>
       </c>
-      <c r="R15" s="8" t="s">
+      <c r="R15" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="2:18">
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="6">
+      <c r="C16" s="5"/>
+      <c r="D16" s="1">
         <v>4</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1">
         <v>10</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6">
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1">
         <v>10</v>
       </c>
-      <c r="K16" s="6"/>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6">
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1">
         <v>13</v>
       </c>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="8"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="5"/>
     </row>
     <row r="17" spans="2:18">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="5"/>
     </row>
     <row r="18" spans="2:18">
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="9">
+      <c r="C18" s="1"/>
+      <c r="D18" s="6">
         <f>SUM(D5:D14)</f>
         <v>66435.22</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="6">
         <f t="shared" ref="E18:Q18" si="1">SUM(E5:E14)</f>
         <v>66353.22</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="6">
         <f t="shared" si="1"/>
         <v>68396.9</v>
       </c>
-      <c r="G18" s="9">
+      <c r="G18" s="6">
         <f t="shared" si="1"/>
         <v>67579.44</v>
       </c>
-      <c r="H18" s="9">
+      <c r="H18" s="6">
         <f t="shared" si="1"/>
         <v>66531.12</v>
       </c>
-      <c r="I18" s="9">
+      <c r="I18" s="6">
         <f t="shared" si="1"/>
         <v>65457.83</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J18" s="6">
         <f t="shared" si="1"/>
         <v>63977.55</v>
       </c>
-      <c r="K18" s="9">
+      <c r="K18" s="6">
         <f t="shared" si="1"/>
         <v>62977.48</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="6">
         <f t="shared" si="1"/>
         <v>64144.2</v>
       </c>
-      <c r="M18" s="9">
+      <c r="M18" s="6">
         <f t="shared" si="1"/>
         <v>65570.62</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="6">
         <f t="shared" si="1"/>
         <v>68307.63</v>
       </c>
-      <c r="O18" s="9">
+      <c r="O18" s="6">
         <f t="shared" si="1"/>
         <v>64658.63</v>
       </c>
-      <c r="P18" s="9">
+      <c r="P18" s="6">
         <f t="shared" si="1"/>
         <v>70800.1</v>
       </c>
-      <c r="Q18" s="9">
+      <c r="Q18" s="6">
         <f t="shared" si="1"/>
         <v>65187.17</v>
       </c>
-      <c r="R18" s="7">
+      <c r="R18" s="4">
         <f>SMALL(D18:Q18,1)</f>
         <v>62977.48</v>
       </c>
@@ -1990,8 +2004,5 @@
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
-  <ignoredErrors>
-    <ignoredError sqref="R5:R14" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>